<commit_message>
Reduced Delay for Job Creation
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Critical_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3489,9 +3489,6 @@
     <t>No.2  Ward No.8456</t>
   </si>
   <si>
-    <t>1707105271</t>
-  </si>
-  <si>
     <t>3543224602</t>
   </si>
   <si>
@@ -3511,6 +3508,9 @@
   </si>
   <si>
     <t>AutoGlobalProduct 04March2020 16:24:02</t>
+  </si>
+  <si>
+    <t>1707105274</t>
   </si>
 </sst>
 </file>
@@ -5982,7 +5982,7 @@
         <v>197</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1136</v>
+        <v>1143</v>
       </c>
       <c r="C2" s="59"/>
       <c r="E2" s="59"/>
@@ -6037,7 +6037,7 @@
         <v>991</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="12" spans="1:167" x14ac:dyDescent="0.25">
@@ -6045,7 +6045,7 @@
         <v>992</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="13" spans="1:167" x14ac:dyDescent="0.25">
@@ -6058,7 +6058,7 @@
         <v>1069</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="15" spans="1:167" x14ac:dyDescent="0.25">
@@ -6066,7 +6066,7 @@
         <v>1070</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="16" spans="1:167" x14ac:dyDescent="0.25">
@@ -6074,7 +6074,7 @@
         <v>1071</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6082,7 +6082,7 @@
         <v>1072</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6090,7 +6090,7 @@
         <v>1073</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -6098,7 +6098,7 @@
         <v>1074</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -6106,7 +6106,7 @@
         <v>1075</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -6114,7 +6114,7 @@
         <v>1076</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -11525,7 +11525,7 @@
         <v>1043</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made Changes to Amend Company Client and Company Brand Added Data sheet and TestManger items
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="46" activeTab="49"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -55,19 +55,25 @@
     <sheet name="Reverse Invoice" sheetId="41" r:id="rId41"/>
     <sheet name="Credit Note With PO" sheetId="42" r:id="rId42"/>
     <sheet name="CreateClient" sheetId="57" r:id="rId43"/>
-    <sheet name="AmendGlobalClient" sheetId="55" r:id="rId44"/>
-    <sheet name="AmendGlobalBrand" sheetId="56" r:id="rId45"/>
-    <sheet name="BlockGlobalClient" sheetId="47" r:id="rId46"/>
-    <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId47"/>
-    <sheet name="BlockCompanyBrand" sheetId="50" r:id="rId48"/>
-    <sheet name="BlockCompanyClient" sheetId="51" r:id="rId49"/>
-    <sheet name="BlockGlobalProduct" sheetId="52" r:id="rId50"/>
-    <sheet name="BlockCompanyProduct" sheetId="53" r:id="rId51"/>
-    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId52"/>
-    <sheet name="CreateGlobalVendor" sheetId="58" r:id="rId53"/>
-    <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId54"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId55"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId56"/>
+    <sheet name="CreateCompanyClient" sheetId="59" r:id="rId44"/>
+    <sheet name="CreateCompanyBrand" sheetId="60" r:id="rId45"/>
+    <sheet name="CreateGlobalBrand" sheetId="63" r:id="rId46"/>
+    <sheet name="CreateGlobalProduct" sheetId="64" r:id="rId47"/>
+    <sheet name="AmendCompanyClient" sheetId="61" r:id="rId48"/>
+    <sheet name="AmendCompanyBrand" sheetId="62" r:id="rId49"/>
+    <sheet name="AmendGlobalClient" sheetId="55" r:id="rId50"/>
+    <sheet name="AmendGlobalBrand" sheetId="56" r:id="rId51"/>
+    <sheet name="BlockGlobalClient" sheetId="47" r:id="rId52"/>
+    <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId53"/>
+    <sheet name="BlockCompanyBrand" sheetId="50" r:id="rId54"/>
+    <sheet name="BlockCompanyClient" sheetId="51" r:id="rId55"/>
+    <sheet name="BlockGlobalProduct" sheetId="52" r:id="rId56"/>
+    <sheet name="BlockCompanyProduct" sheetId="53" r:id="rId57"/>
+    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId58"/>
+    <sheet name="CreateGlobalVendor" sheetId="58" r:id="rId59"/>
+    <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId60"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId61"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId62"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -79,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1174">
   <si>
     <t>Description</t>
   </si>
@@ -3511,6 +3517,96 @@
   </si>
   <si>
     <t>1707105274</t>
+  </si>
+  <si>
+    <t>1712_INR_Billable_Price_List</t>
+  </si>
+  <si>
+    <t>JobPricelListSales</t>
+  </si>
+  <si>
+    <t>25 Days</t>
+  </si>
+  <si>
+    <t>ControlAccountNo</t>
+  </si>
+  <si>
+    <t>17129905</t>
+  </si>
+  <si>
+    <t>AccountDirectorNo</t>
+  </si>
+  <si>
+    <t>matheww@oglivy.com</t>
+  </si>
+  <si>
+    <t>mathew@oglivy.com</t>
+  </si>
+  <si>
+    <t>mathew</t>
+  </si>
+  <si>
+    <t>1712</t>
+  </si>
+  <si>
+    <t>Settling company</t>
+  </si>
+  <si>
+    <t>1707_AutoClient 24February2020 15:20:12</t>
+  </si>
+  <si>
+    <t>Testo India Private Limited</t>
+  </si>
+  <si>
+    <t>107734</t>
+  </si>
+  <si>
+    <t>107739</t>
+  </si>
+  <si>
+    <t>AutoGlobalBrand 24February2020 16:44:49</t>
+  </si>
+  <si>
+    <t>1707_AutoClient 24February2020 16:44:49</t>
+  </si>
+  <si>
+    <t>107738001</t>
+  </si>
+  <si>
+    <t>107738</t>
+  </si>
+  <si>
+    <t>contact@mdfiindia.com</t>
+  </si>
+  <si>
+    <t>+91 2261083101</t>
+  </si>
+  <si>
+    <t>contact@mdndia.com</t>
+  </si>
+  <si>
+    <t>+91 2261083232</t>
+  </si>
+  <si>
+    <t>cok111</t>
+  </si>
+  <si>
+    <t>Default Name</t>
+  </si>
+  <si>
+    <t>Pepsi1</t>
+  </si>
+  <si>
+    <t>3543214642</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Pespi</t>
+  </si>
+  <si>
+    <t>c1011</t>
   </si>
 </sst>
 </file>
@@ -3784,7 +3880,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3987,6 +4083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11438,8 +11535,8 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11675,179 +11772,389 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="106" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="106" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>984</v>
       </c>
-      <c r="B2" s="59" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="59" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>236</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="59" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1154</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B8" s="100" t="s">
-        <v>1134</v>
+        <v>1095</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="100" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C9" s="100" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>974</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1055</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="C9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="106" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="106" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>984</v>
       </c>
-      <c r="B2" s="59" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B3" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="59" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>985</v>
       </c>
-      <c r="B4" s="102" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="59"/>
+      <c r="C4" s="59" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>986</v>
       </c>
-      <c r="B5" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="59"/>
+      <c r="C6" s="59" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>375</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1154</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>372</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B10" s="100" t="s">
-        <v>1128</v>
+        <v>1095</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C11" s="100" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>974</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1055</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11856,16 +12163,16 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11878,23 +12185,250 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>984</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>1112</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>984</v>
+      </c>
+      <c r="B4">
+        <v>107742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>986</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>236</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B14" t="s">
         <v>375</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B19" s="100" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B21">
+        <v>17079905</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B28">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B30">
+        <v>464576457</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B31">
+        <v>34576457</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11903,16 +12437,16 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11925,39 +12459,255 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>984</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>1115</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>1033</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>985</v>
-      </c>
-      <c r="B4" s="102" t="s">
-        <v>1114</v>
+        <v>984</v>
+      </c>
+      <c r="B4">
+        <v>107742</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>986</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1126</v>
+        <v>985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>998</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B20" s="100" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B21" s="59" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B22">
+        <v>17079905</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B31">
+        <v>464576457</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B32">
+        <v>34576457</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B20" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11969,21 +12719,21 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101">
-        <v>1707</v>
+      <c r="B1" s="50" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -11991,7 +12741,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="104" t="s">
-        <v>993</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -12004,23 +12754,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>985</v>
-      </c>
-      <c r="B4" s="102" t="s">
-        <v>994</v>
+        <v>1022</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>1164</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>986</v>
-      </c>
-      <c r="B5" t="s">
-        <v>995</v>
+        <v>1023</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12029,16 +12779,16 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12054,7 +12804,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="104" t="s">
-        <v>993</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -12065,9 +12815,41 @@
         <v>375</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>985</v>
+      </c>
+      <c r="B6" s="102" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>986</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12337,6 +13119,404 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="101">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B8" s="100" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="101">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>985</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>986</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B10" s="100" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="101">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="101">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>985</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>986</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="101">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>985</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>986</v>
+      </c>
+      <c r="B5" t="s">
+        <v>995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12395,7 +13575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12458,7 +13638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12521,7 +13701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12816,467 +13996,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>987</v>
-      </c>
-      <c r="B2">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>988</v>
-      </c>
-      <c r="B3">
-        <v>107444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>989</v>
-      </c>
-      <c r="B4" s="103" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="37">
-        <v>1707</v>
-      </c>
-      <c r="C1" s="37">
-        <v>1712</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="95" t="s">
-        <v>942</v>
-      </c>
-      <c r="C2" s="95" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="95" t="s">
-        <v>943</v>
-      </c>
-      <c r="C3" s="95" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="95" t="s">
-        <v>944</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="95" t="s">
-        <v>945</v>
-      </c>
-      <c r="C5" s="95" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="95" t="s">
-        <v>362</v>
-      </c>
-      <c r="C6" s="95" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="95" t="s">
-        <v>946</v>
-      </c>
-      <c r="C7" s="95" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="95" t="s">
-        <v>947</v>
-      </c>
-      <c r="C8" s="95" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="95" t="s">
-        <v>948</v>
-      </c>
-      <c r="C9" s="95" t="s">
-        <v>1123</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="95" t="s">
-        <v>949</v>
-      </c>
-      <c r="C10" s="95" t="s">
-        <v>1124</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B11" s="96" t="s">
-        <v>950</v>
-      </c>
-      <c r="C11" s="96" t="s">
-        <v>1125</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="98" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="95" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="95" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="95" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="95" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="95" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="96" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="99" t="s">
-        <v>967</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13417,6 +14136,467 @@
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>988</v>
+      </c>
+      <c r="B3">
+        <v>107444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>989</v>
+      </c>
+      <c r="B4" s="103" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="37">
+        <v>1707</v>
+      </c>
+      <c r="C1" s="37">
+        <v>1712</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="95" t="s">
+        <v>942</v>
+      </c>
+      <c r="C2" s="95" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>943</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="95" t="s">
+        <v>944</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>945</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="95" t="s">
+        <v>362</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>946</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="95" t="s">
+        <v>947</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>948</v>
+      </c>
+      <c r="C9" s="95" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>949</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="96" t="s">
+        <v>950</v>
+      </c>
+      <c r="C11" s="96" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="98" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="95" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="95" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="95" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="95" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="95" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="95" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="96" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>967</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Company Vendor with Data Sheet And Name mapping
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="46" activeTab="49"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="40" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -63,17 +63,20 @@
     <sheet name="AmendCompanyBrand" sheetId="62" r:id="rId49"/>
     <sheet name="AmendGlobalClient" sheetId="55" r:id="rId50"/>
     <sheet name="AmendGlobalBrand" sheetId="56" r:id="rId51"/>
-    <sheet name="BlockGlobalClient" sheetId="47" r:id="rId52"/>
-    <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId53"/>
-    <sheet name="BlockCompanyBrand" sheetId="50" r:id="rId54"/>
-    <sheet name="BlockCompanyClient" sheetId="51" r:id="rId55"/>
-    <sheet name="BlockGlobalProduct" sheetId="52" r:id="rId56"/>
-    <sheet name="BlockCompanyProduct" sheetId="53" r:id="rId57"/>
-    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId58"/>
-    <sheet name="CreateGlobalVendor" sheetId="58" r:id="rId59"/>
-    <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId60"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId61"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId62"/>
+    <sheet name="AmendGlobalVendor" sheetId="65" r:id="rId52"/>
+    <sheet name="AmendCompanyVendor" sheetId="66" r:id="rId53"/>
+    <sheet name="BlockGlobalClient" sheetId="47" r:id="rId54"/>
+    <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId55"/>
+    <sheet name="BlockCompanyBrand" sheetId="50" r:id="rId56"/>
+    <sheet name="BlockCompanyClient" sheetId="51" r:id="rId57"/>
+    <sheet name="BlockGlobalProduct" sheetId="52" r:id="rId58"/>
+    <sheet name="BlockCompanyProduct" sheetId="53" r:id="rId59"/>
+    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId60"/>
+    <sheet name="CreateGlobalVendor" sheetId="58" r:id="rId61"/>
+    <sheet name="CreateCompanyVendor" sheetId="67" r:id="rId62"/>
+    <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId63"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId64"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId65"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -85,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="1184">
   <si>
     <t>Description</t>
   </si>
@@ -3607,6 +3610,36 @@
   </si>
   <si>
     <t>c1011</t>
+  </si>
+  <si>
+    <t>GlobalVendor_1</t>
+  </si>
+  <si>
+    <t>Global1@yahoo.com</t>
+  </si>
+  <si>
+    <t>TaxNo</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Global@gmail.com</t>
+  </si>
+  <si>
+    <t>Payment Mode</t>
+  </si>
+  <si>
+    <t>IN - NEFT - 1</t>
+  </si>
+  <si>
+    <t>Settling_Company</t>
+  </si>
+  <si>
+    <t>Global@yahoo.com</t>
+  </si>
+  <si>
+    <t>BRISK OFFICE AUTOMATION</t>
   </si>
 </sst>
 </file>
@@ -11536,7 +11569,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11774,8 +11807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13121,7 +13154,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -13297,6 +13330,164 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="100" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B5">
+        <v>9586786246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B6" s="59">
+        <v>84625318710</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B7" s="59">
+        <v>84625318710</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B4">
+        <v>958647231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13339,7 +13530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -13402,7 +13593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -13465,7 +13656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -13512,7 +13703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -13575,7 +13766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -13635,367 +13826,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>987</v>
-      </c>
-      <c r="B2">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3">
-        <v>107433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B4" s="103" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B34"/>
-  <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1035</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="100" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B5">
-        <v>9683254705</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1078</v>
-      </c>
-      <c r="B8">
-        <v>6000056</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1079</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1083</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1086</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1089</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1092</v>
-      </c>
-      <c r="B19" s="59" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>235</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>1097</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B27">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>1103</v>
-      </c>
-      <c r="B28">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>1104</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1107</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>1108</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>1110</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>313</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14151,6 +13981,502 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3">
+        <v>107433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="103" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="100" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B5">
+        <v>9683254705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B8">
+        <v>6000056</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B27">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B28">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B4">
+        <v>9846201537</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B13">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -14206,7 +14532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -14461,7 +14787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>

</xml_diff>

<commit_message>
Create Budget is updated
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1180">
   <si>
     <t>Description</t>
   </si>
@@ -3504,15 +3504,9 @@
     <t>AutoGlobalBrand 04March2020 16:24:02</t>
   </si>
   <si>
-    <t>107762001001</t>
-  </si>
-  <si>
     <t>AutoGlobalProduct 04March2020 16:24:02</t>
   </si>
   <si>
-    <t>1707105274</t>
-  </si>
-  <si>
     <t>1712_INR_Billable_Price_List</t>
   </si>
   <si>
@@ -3631,6 +3625,9 @@
   </si>
   <si>
     <t>BRISK OFFICE AUTOMATION</t>
+  </si>
+  <si>
+    <t>1707105275</t>
   </si>
 </sst>
 </file>
@@ -5912,8 +5909,8 @@
   </sheetPr>
   <dimension ref="A1:FK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,7 +6100,7 @@
         <v>197</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1140</v>
+        <v>1179</v>
       </c>
       <c r="C2" s="59"/>
       <c r="E2" s="59"/>
@@ -6210,16 +6207,13 @@
       <c r="A18" s="30" t="s">
         <v>1070</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>1138</v>
-      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>1071</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11817,7 +11811,7 @@
         <v>370</v>
       </c>
       <c r="C1" s="106" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -11842,10 +11836,10 @@
         <v>982</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -11853,10 +11847,10 @@
         <v>1030</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -11872,13 +11866,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>370</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -11897,10 +11891,10 @@
         <v>1092</v>
       </c>
       <c r="B8" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C8" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -11908,26 +11902,26 @@
         <v>29</v>
       </c>
       <c r="B9" s="100" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C9" s="100" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>972</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B11" t="s">
         <v>1044</v>
@@ -11941,21 +11935,21 @@
         <v>1095</v>
       </c>
       <c r="B12" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C12" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>1054</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -12002,7 +11996,7 @@
         <v>370</v>
       </c>
       <c r="C1" s="106" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -12027,10 +12021,10 @@
         <v>982</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -12039,7 +12033,7 @@
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12047,10 +12041,10 @@
         <v>1030</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -12059,7 +12053,7 @@
       </c>
       <c r="B6" s="59"/>
       <c r="C6" s="59" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -12075,13 +12069,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>370</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -12100,10 +12094,10 @@
         <v>1092</v>
       </c>
       <c r="B10" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C10" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -12111,26 +12105,26 @@
         <v>29</v>
       </c>
       <c r="B11" s="100" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>972</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="B13" t="s">
         <v>1044</v>
@@ -12144,21 +12138,21 @@
         <v>1095</v>
       </c>
       <c r="B14" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C14" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>1054</v>
       </c>
       <c r="C15" s="59" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -12236,15 +12230,15 @@
         <v>984</v>
       </c>
       <c r="B5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B6" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -12300,7 +12294,7 @@
         <v>1040</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -12393,10 +12387,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B25" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -12515,15 +12509,15 @@
         <v>996</v>
       </c>
       <c r="B6" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B7" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -12579,7 +12573,7 @@
         <v>1040</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -12672,10 +12666,10 @@
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B26" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -12781,7 +12775,7 @@
         <v>1019</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12789,7 +12783,7 @@
         <v>1020</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
@@ -12844,7 +12838,7 @@
         <v>1019</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12852,7 +12846,7 @@
         <v>1020</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -13351,7 +13345,7 @@
         <v>1000</v>
       </c>
       <c r="B3" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13359,7 +13353,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -13380,7 +13374,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B7" s="59">
         <v>84625318710</v>
@@ -13388,7 +13382,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B8" t="s">
         <v>373</v>
@@ -13438,7 +13432,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="100" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13451,7 +13445,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B5" t="s">
         <v>373</v>
@@ -13459,10 +13453,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="B6" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
   </sheetData>
@@ -14349,7 +14343,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1003</v>
@@ -14360,7 +14354,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="100" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14424,7 +14418,7 @@
         <v>1000</v>
       </c>
       <c r="B11" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Namemapping change - Create Global Brand
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="40" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="43" activeTab="45"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="1175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="1177">
   <si>
     <t>Description</t>
   </si>
@@ -3540,9 +3540,6 @@
     <t>+91 2261083232</t>
   </si>
   <si>
-    <t>cok111</t>
-  </si>
-  <si>
     <t>Default Name</t>
   </si>
   <si>
@@ -3613,6 +3610,15 @@
   </si>
   <si>
     <t>3543245765</t>
+  </si>
+  <si>
+    <t>107742</t>
+  </si>
+  <si>
+    <t>cok1112</t>
+  </si>
+  <si>
+    <t>3543215664</t>
   </si>
 </sst>
 </file>
@@ -4407,48 +4413,59 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="73">
         <v>1707</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="73">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="94" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="94" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="71" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6120,7 +6137,7 @@
         <v>197</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C2" s="59"/>
       <c r="E2" s="59"/>
@@ -11573,7 +11590,7 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -11652,7 +11669,7 @@
         <v>1033</v>
       </c>
       <c r="B9" s="120" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -11660,7 +11677,7 @@
         <v>1035</v>
       </c>
       <c r="B10" s="120" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -12203,8 +12220,8 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12241,8 +12258,8 @@
       <c r="A4" t="s">
         <v>982</v>
       </c>
-      <c r="B4">
-        <v>107742</v>
+      <c r="B4" s="120" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12250,15 +12267,15 @@
         <v>984</v>
       </c>
       <c r="B5" t="s">
-        <v>1150</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B6" t="s">
         <v>1151</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -12313,8 +12330,8 @@
       <c r="A13" t="s">
         <v>1035</v>
       </c>
-      <c r="B13" s="59" t="s">
-        <v>1153</v>
+      <c r="B13" s="120" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -12407,10 +12424,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B25" t="s">
         <v>1154</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -12529,15 +12546,15 @@
         <v>992</v>
       </c>
       <c r="B6" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B7" t="s">
         <v>1151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -12593,7 +12610,7 @@
         <v>1035</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -12686,10 +12703,10 @@
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B26" t="s">
         <v>1154</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -13368,7 +13385,7 @@
         <v>996</v>
       </c>
       <c r="B3" s="118" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13376,7 +13393,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -13397,7 +13414,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="118" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B7" s="120">
         <v>846253110</v>
@@ -13405,7 +13422,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="118" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B8" s="118" t="s">
         <v>373</v>
@@ -13458,7 +13475,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="117" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13471,7 +13488,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="115" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B5" s="115" t="s">
         <v>373</v>
@@ -13479,10 +13496,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="115" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B6" s="115" t="s">
         <v>1159</v>
-      </c>
-      <c r="B6" s="115" t="s">
-        <v>1160</v>
       </c>
     </row>
   </sheetData>
@@ -14022,7 +14039,7 @@
         <v>996</v>
       </c>
       <c r="B3" s="122" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14077,7 +14094,7 @@
         <v>1027</v>
       </c>
       <c r="B3" s="111" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14085,7 +14102,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -14109,7 +14126,7 @@
         <v>996</v>
       </c>
       <c r="B7" s="111" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -14181,7 +14198,7 @@
         <v>1079</v>
       </c>
       <c r="B16" s="111" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -14205,7 +14222,7 @@
         <v>1083</v>
       </c>
       <c r="B19" s="113" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -14361,7 +14378,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B2" s="109" t="s">
         <v>997</v>
@@ -14372,7 +14389,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="110" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14436,7 +14453,7 @@
         <v>996</v>
       </c>
       <c r="B11" s="108" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Amended Company vendor and Datasheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="1182">
   <si>
     <t>Description</t>
   </si>
@@ -5954,8 +5954,8 @@
   </sheetPr>
   <dimension ref="A1:FK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6303,8 +6303,11 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="121" t="s">
         <v>996</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>1175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script updation CreateAGeneralJournal and ReverseAGeneralJournal
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="62" activeTab="63"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -5988,8 +5988,8 @@
   </sheetPr>
   <dimension ref="A1:FK23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14635,7 +14635,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified Batch 5 scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegPack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="63" activeTab="64"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="1206">
   <si>
     <t>Description</t>
   </si>
@@ -3692,9 +3692,6 @@
     <t>General Journal No</t>
   </si>
   <si>
-    <t>1707117425</t>
-  </si>
-  <si>
     <t>JournalNo</t>
   </si>
   <si>
@@ -3702,6 +3699,15 @@
   </si>
   <si>
     <t>03/13/2020</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>Payable</t>
+  </si>
+  <si>
+    <t>1707117445</t>
   </si>
 </sst>
 </file>
@@ -4475,7 +4481,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -5994,7 +6000,7 @@
   <dimension ref="A1:FK24"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6349,7 +6355,7 @@
         <v>1199</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>1200</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -6741,7 +6747,7 @@
   <dimension ref="A1:BL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14669,16 +14675,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="108" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B2" s="109"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="108" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B3" s="110" t="s">
         <v>1202</v>
-      </c>
-      <c r="B3" s="110" t="s">
-        <v>1203</v>
       </c>
     </row>
   </sheetData>
@@ -14692,10 +14698,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14703,15 +14709,17 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1183</v>
       </c>
@@ -14725,69 +14733,114 @@
         <v>1190</v>
       </c>
       <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
         <v>337</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1184</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1185</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1186</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1187</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" t="s">
         <v>338</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>1191</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>1192</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>131</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>1193</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>1194</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1708</v>
+      </c>
+      <c r="F2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>1197</v>
+      </c>
+      <c r="J2" s="59"/>
+      <c r="K2">
+        <v>500</v>
+      </c>
+      <c r="M2" t="s">
+        <v>344</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="P2" s="59" t="s">
+        <v>1198</v>
+      </c>
+      <c r="Q2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1707</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>372</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>1197</v>
+      </c>
+      <c r="J3" s="59"/>
+      <c r="K3">
+        <v>500</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="M3" t="s">
         <v>344</v>
       </c>
-      <c r="G2" t="s">
-        <v>1195</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I2" s="59"/>
-      <c r="J2">
-        <v>500</v>
-      </c>
-      <c r="K2" t="s">
-        <v>344</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O3" t="s">
         <v>1196</v>
       </c>
-      <c r="N2" s="59" t="s">
+      <c r="P3" s="59" t="s">
         <v>1198</v>
       </c>
-      <c r="O2">
+      <c r="Q3">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Import Budget Model, DataSheet , NameMapping
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\741496\Documents\bau_environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="62" activeTab="65"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="63" activeTab="66"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -78,8 +78,9 @@
     <sheet name="ReverseGL" sheetId="69" r:id="rId64"/>
     <sheet name="CreateGeneralJournal" sheetId="68" r:id="rId65"/>
     <sheet name="CreateReversingGeneralJournal" sheetId="70" r:id="rId66"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId67"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId68"/>
+    <sheet name="ImportBudgetModel" sheetId="71" r:id="rId67"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId68"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId69"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="1201">
   <si>
     <t>Description</t>
   </si>
@@ -3683,6 +3684,18 @@
   </si>
   <si>
     <t>1010000-06</t>
+  </si>
+  <si>
+    <t>Job_Department</t>
+  </si>
+  <si>
+    <t>RB101</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>-2500.00</t>
   </si>
 </sst>
 </file>
@@ -3956,7 +3969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4171,6 +4184,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14971,7 +14986,7 @@
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -15098,6 +15113,66 @@
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="112" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B5" s="113" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -15351,7 +15426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>

</xml_diff>

<commit_message>
Added Batch 5 scripts. Namemapping and Datasheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegPack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Documents\Results\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="62" activeTab="65"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,12 @@
     <sheet name="CreateCompanyVendor" sheetId="67" r:id="rId63"/>
     <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId64"/>
     <sheet name="ReverseGL" sheetId="69" r:id="rId65"/>
-    <sheet name="CreateGeneralJournal" sheetId="68" r:id="rId66"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId67"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId68"/>
+    <sheet name="CreateCurrencyJournal" sheetId="71" r:id="rId66"/>
+    <sheet name="CopyGL" sheetId="72" r:id="rId67"/>
+    <sheet name="ReverseGL (2)" sheetId="73" r:id="rId68"/>
+    <sheet name="CreateGeneralJournal" sheetId="68" r:id="rId69"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId70"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId71"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -91,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1217">
   <si>
     <t>Description</t>
   </si>
@@ -3731,6 +3734,18 @@
   </si>
   <si>
     <t>1707109754</t>
+  </si>
+  <si>
+    <t>04/13/2020</t>
+  </si>
+  <si>
+    <t>CreatedOn</t>
+  </si>
+  <si>
+    <t>3/17/2020</t>
+  </si>
+  <si>
+    <t>01/13/2020</t>
   </si>
 </sst>
 </file>
@@ -4004,7 +4019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4218,6 +4233,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14777,6 +14793,146 @@
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="107">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="109">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B4" s="111" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="107">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B2" s="109"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="108" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="108" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="108"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="107">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B2" s="109"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B3" s="110" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
@@ -14932,404 +15088,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="37">
-        <v>1707</v>
-      </c>
-      <c r="C1" s="37">
-        <v>1712</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>940</v>
-      </c>
-      <c r="C2" s="94" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="94" t="s">
-        <v>941</v>
-      </c>
-      <c r="C3" s="94" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="94" t="s">
-        <v>942</v>
-      </c>
-      <c r="C4" s="94" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="94" t="s">
-        <v>943</v>
-      </c>
-      <c r="C5" s="94" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="94" t="s">
-        <v>362</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="94" t="s">
-        <v>944</v>
-      </c>
-      <c r="C7" s="94" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="94" t="s">
-        <v>945</v>
-      </c>
-      <c r="C8" s="94" t="s">
-        <v>1118</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="94" t="s">
-        <v>946</v>
-      </c>
-      <c r="C9" s="94" t="s">
-        <v>1119</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="94" t="s">
-        <v>947</v>
-      </c>
-      <c r="C10" s="94" t="s">
-        <v>1120</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B11" s="95" t="s">
-        <v>948</v>
-      </c>
-      <c r="C11" s="95" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="97" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="94" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="95" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="98" t="s">
-        <v>965</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -15337,7 +15095,7 @@
   </sheetPr>
   <dimension ref="A1:BJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -15643,6 +15401,404 @@
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1707</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="37">
+        <v>1707</v>
+      </c>
+      <c r="C1" s="37">
+        <v>1712</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>940</v>
+      </c>
+      <c r="C2" s="94" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="94" t="s">
+        <v>941</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>942</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>943</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>362</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>944</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="94" t="s">
+        <v>945</v>
+      </c>
+      <c r="C8" s="94" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="94" t="s">
+        <v>946</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="94" t="s">
+        <v>947</v>
+      </c>
+      <c r="C10" s="94" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="95" t="s">
+        <v>948</v>
+      </c>
+      <c r="C11" s="95" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="94" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="94" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="94" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="94" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="94" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="95" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="98" t="s">
+        <v>965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized Create Budget and Batch 6 scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Documents\Results\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="62" activeTab="65"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="66" activeTab="69"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -81,8 +81,9 @@
     <sheet name="CopyGL" sheetId="72" r:id="rId67"/>
     <sheet name="ReverseGL (2)" sheetId="73" r:id="rId68"/>
     <sheet name="CreateGeneralJournal" sheetId="68" r:id="rId69"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId70"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId71"/>
+    <sheet name="InvoicePreparation" sheetId="74" r:id="rId70"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId71"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId72"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="1218">
   <si>
     <t>Description</t>
   </si>
@@ -3746,6 +3747,9 @@
   </si>
   <si>
     <t>01/13/2020</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -14795,7 +14799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -15412,6 +15416,53 @@
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:M11"/>
@@ -15664,7 +15715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>

</xml_diff>

<commit_message>
Updated Regression JIRA ID
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="106" activeTab="106"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="25" activeTab="106"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -4468,7 +4468,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5282,9 +5281,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5368,9 +5367,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5590,7 +5589,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5625,15 +5624,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5730,13 +5729,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5827,16 +5826,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5964,51 +5963,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="65" max="65" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="15" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" x14ac:dyDescent="0.25">
@@ -6694,13 +6693,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6762,8 +6761,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6822,10 +6821,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="106" width="23.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="106" width="24.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="106" width="22.28515625" collapsed="true"/>
-    <col min="5" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="2" width="23" style="106" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="106" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.28515625" style="106" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6970,9 +6969,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7192,10 +7191,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="22.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="106" width="29.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="106" width="34.140625" collapsed="true"/>
-    <col min="4" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.7109375" style="106" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.140625" style="106" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7301,9 +7300,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="15.5703125" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7394,9 +7393,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -7530,9 +7529,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7606,9 +7605,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7665,9 +7664,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7724,9 +7723,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="106" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="106" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7783,8 +7782,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7838,9 +7837,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="3" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8072,8 +8071,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8215,10 +8214,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="49" width="30.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="49" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="26.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.140625" style="49" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8359,40 +8358,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="56" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
@@ -8739,41 +8738,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -9129,41 +9128,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -9519,41 +9518,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -9909,41 +9908,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -10299,41 +10298,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -10645,48 +10644,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
@@ -10938,7 +10937,7 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FK42"/>
+  <dimension ref="A1:FK43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -10946,12 +10945,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="26.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="36.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="30" width="36.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="30" width="40.0" collapsed="true"/>
-    <col min="5" max="167" customWidth="true" style="30" width="32.0" collapsed="true"/>
-    <col min="168" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="26" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40" style="30" customWidth="1" collapsed="1"/>
+    <col min="5" max="167" width="32" style="30" customWidth="1" collapsed="1"/>
+    <col min="168" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:167" x14ac:dyDescent="0.25">
@@ -11500,7 +11499,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1426</v>
       </c>
@@ -11527,8 +11526,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" style="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11694,16 +11693,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="60.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="59.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="30" width="51.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="30" width="51.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="30" width="58.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="30" width="57.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="30" width="63.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="30" width="45.28515625" collapsed="true"/>
-    <col min="10" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="58.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="63.7109375" style="30" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.28515625" style="30" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12050,9 +12049,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="23.140625" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12146,11 +12145,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="68.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="67.42578125" collapsed="true"/>
-    <col min="4" max="9" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="69.42578125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="9" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12587,8 +12586,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12717,8 +12716,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="46.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12828,9 +12827,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -12958,11 +12957,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="30" width="8.5703125" collapsed="true"/>
-    <col min="5" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -13020,9 +13019,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -13079,9 +13078,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -13138,7 +13137,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="12" style="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14456,9 +14455,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -14515,9 +14514,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -14574,9 +14573,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -14621,8 +14620,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14658,8 +14657,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -14703,8 +14702,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14739,8 +14738,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14790,8 +14789,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14841,57 +14840,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="72" max="73" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="72" max="73" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.25">
@@ -15187,51 +15186,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="22" max="23" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="28" max="29" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="34" max="35" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="40" max="41" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="46" max="47" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="53" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="58" max="59" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="64" max="65" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="53" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="58" max="59" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="64" max="65" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
@@ -15463,7 +15462,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17517,52 +17516,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -17806,52 +17805,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -18095,52 +18094,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -18384,52 +18383,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -18673,52 +18672,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="30" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -18962,8 +18961,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -18999,8 +18998,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19044,8 +19043,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19089,8 +19088,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19134,8 +19133,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19179,8 +19178,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -19257,8 +19256,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19302,8 +19301,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19339,8 +19338,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19434,10 +19433,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="16.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="12.42578125" collapsed="true"/>
-    <col min="4" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19507,8 +19506,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19578,8 +19577,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19649,8 +19648,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19720,11 +19719,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -19789,13 +19788,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -19872,13 +19871,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -19955,10 +19954,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="30" width="31.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.85546875" style="30" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.42578125" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20192,13 +20191,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -20275,7 +20274,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -20314,7 +20313,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20358,7 +20357,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20394,8 +20393,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20443,8 +20442,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20494,9 +20493,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20557,9 +20556,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20628,8 +20627,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20674,9 +20673,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20740,9 +20739,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -20968,17 +20967,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -21117,9 +21116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="15.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -21197,8 +21196,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -21268,11 +21267,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -21454,8 +21453,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -21698,9 +21697,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -21886,9 +21885,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -22092,8 +22091,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -22366,8 +22365,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -22645,8 +22644,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -22708,9 +22707,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -22936,8 +22935,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23015,8 +23014,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23096,8 +23095,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23193,8 +23192,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23280,8 +23279,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23351,8 +23350,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23398,8 +23397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23461,8 +23460,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23524,8 +23523,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23571,8 +23570,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23634,9 +23633,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23862,8 +23861,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23925,8 +23924,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23988,8 +23987,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24286,8 +24285,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24424,8 +24423,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24487,9 +24486,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="106" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="106" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="106" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="106" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="106" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24530,8 +24529,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24566,8 +24565,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24611,17 +24610,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -24769,17 +24768,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Data Sheet updated - SubJob
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\3D Objects\Git Project New\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="108" activeTab="118"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4001" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="1481">
   <si>
     <t>Description</t>
   </si>
@@ -4579,6 +4579,21 @@
   </si>
   <si>
     <t>8/8/2020</t>
+  </si>
+  <si>
+    <t>1707106464</t>
+  </si>
+  <si>
+    <t>1707_TestAutomation_07072020</t>
+  </si>
+  <si>
+    <t>7/6/2020</t>
+  </si>
+  <si>
+    <t>Job_name_Template</t>
+  </si>
+  <si>
+    <t>1707_TestAutomationSubJob</t>
   </si>
 </sst>
 </file>
@@ -8436,7 +8451,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -8513,10 +8528,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8531,120 +8546,162 @@
       <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="2">
+        <v>1707</v>
+      </c>
       <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="7">
+        <v>1707</v>
+      </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="7" t="s">
+        <v>764</v>
+      </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="48" t="s">
+        <v>1476</v>
+      </c>
       <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="7" t="s">
+        <v>766</v>
+      </c>
       <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="44"/>
+      <c r="B7" s="8" t="s">
+        <v>767</v>
+      </c>
       <c r="C7" s="44"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="44"/>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="45"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="45"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="C11" s="44"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="7" t="s">
+        <v>178</v>
+      </c>
       <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="8" t="s">
+        <v>276</v>
+      </c>
       <c r="C13" s="44"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="7" t="s">
+        <v>1067</v>
+      </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="32" t="s">
+        <v>1068</v>
+      </c>
       <c r="C15" s="15"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="32" t="s">
+        <v>1477</v>
+      </c>
       <c r="C16" s="47"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="48" t="s">
+        <v>1478</v>
+      </c>
       <c r="C17" s="48"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>1480</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Direct Debit Ind Excel
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\WPP Global TestScripts\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="71" activeTab="74"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="130" activeTab="133"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -124,33 +124,35 @@
     <sheet name="InvoicePlansDirectInvoice" sheetId="130" r:id="rId110"/>
     <sheet name="InvoicingCarryForward" sheetId="131" r:id="rId111"/>
     <sheet name="JobInvoice_WithoutWIP" sheetId="132" r:id="rId112"/>
-    <sheet name="InvoicingWriteOff" sheetId="79" r:id="rId113"/>
-    <sheet name="CombinedInvoice" sheetId="149" r:id="rId114"/>
-    <sheet name="QuoteMPL" sheetId="111" r:id="rId115"/>
-    <sheet name="InvoiceMPL" sheetId="113" r:id="rId116"/>
-    <sheet name="Time_Material_Invocing" sheetId="150" r:id="rId117"/>
-    <sheet name="JobEstimateMPL" sheetId="147" r:id="rId118"/>
-    <sheet name="AbsenceAllowanceRequest" sheetId="120" r:id="rId119"/>
-    <sheet name="RejectAllowanceRequest" sheetId="115" r:id="rId120"/>
-    <sheet name="ApproveAllowanceRequest" sheetId="114" r:id="rId121"/>
-    <sheet name="ChangePaymentSelection" sheetId="116" r:id="rId122"/>
-    <sheet name="PrintPaymentRemittance" sheetId="117" r:id="rId123"/>
-    <sheet name="CreatePaymentSelection" sheetId="118" r:id="rId124"/>
-    <sheet name="CreatePaymentFile" sheetId="119" r:id="rId125"/>
-    <sheet name="AbsenceRequest" sheetId="122" r:id="rId126"/>
-    <sheet name="RejectAbsence" sheetId="124" r:id="rId127"/>
-    <sheet name="ApproveAbsence" sheetId="123" r:id="rId128"/>
-    <sheet name="CreateAnAccrualJobByJob" sheetId="134" r:id="rId129"/>
-    <sheet name="CreateAnAccrualForAGroupOfJobs" sheetId="135" r:id="rId130"/>
-    <sheet name="ReallocateJobEntries" sheetId="133" r:id="rId131"/>
-    <sheet name="EmailRemittance" sheetId="121" r:id="rId132"/>
-    <sheet name="ImportBudgetModel" sheetId="136" r:id="rId133"/>
-    <sheet name="TimeMPL" sheetId="137" r:id="rId134"/>
-    <sheet name="Modify budget" sheetId="138" r:id="rId135"/>
-    <sheet name="Copy budget" sheetId="139" r:id="rId136"/>
-    <sheet name="ExpensesMPL" sheetId="140" r:id="rId137"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId138"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId139"/>
+    <sheet name="Job Crediting" sheetId="151" r:id="rId113"/>
+    <sheet name="InvoicingWriteOff" sheetId="79" r:id="rId114"/>
+    <sheet name="CombinedInvoice" sheetId="149" r:id="rId115"/>
+    <sheet name="QuoteMPL" sheetId="111" r:id="rId116"/>
+    <sheet name="InvoiceMPL" sheetId="113" r:id="rId117"/>
+    <sheet name="Time_Material_Invocing" sheetId="150" r:id="rId118"/>
+    <sheet name="JobEstimateMPL" sheetId="147" r:id="rId119"/>
+    <sheet name="AbsenceAllowanceRequest" sheetId="120" r:id="rId120"/>
+    <sheet name="RejectAllowanceRequest" sheetId="115" r:id="rId121"/>
+    <sheet name="ApproveAllowanceRequest" sheetId="114" r:id="rId122"/>
+    <sheet name="ChangePaymentSelection" sheetId="116" r:id="rId123"/>
+    <sheet name="PrintPaymentRemittance" sheetId="117" r:id="rId124"/>
+    <sheet name="CreatePaymentSelection" sheetId="118" r:id="rId125"/>
+    <sheet name="CreatePaymentFile" sheetId="119" r:id="rId126"/>
+    <sheet name="AbsenceRequest" sheetId="122" r:id="rId127"/>
+    <sheet name="RejectAbsence" sheetId="124" r:id="rId128"/>
+    <sheet name="ApproveAbsence" sheetId="123" r:id="rId129"/>
+    <sheet name="CreateAnAccrualJobByJob" sheetId="134" r:id="rId130"/>
+    <sheet name="CreateAnAccrualForAGroupOfJobs" sheetId="135" r:id="rId131"/>
+    <sheet name="ReallocateJobEntries" sheetId="133" r:id="rId132"/>
+    <sheet name="EmailRemittance" sheetId="121" r:id="rId133"/>
+    <sheet name="DirectDebitFile" sheetId="152" r:id="rId134"/>
+    <sheet name="ImportBudgetModel" sheetId="136" r:id="rId135"/>
+    <sheet name="TimeMPL" sheetId="137" r:id="rId136"/>
+    <sheet name="Modify budget" sheetId="138" r:id="rId137"/>
+    <sheet name="Copy budget" sheetId="139" r:id="rId138"/>
+    <sheet name="ExpensesMPL" sheetId="140" r:id="rId139"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId140"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId141"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -162,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4631" uniqueCount="1598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4690" uniqueCount="1635">
   <si>
     <t>Description</t>
   </si>
@@ -4786,18 +4788,12 @@
     <t>60,000.00</t>
   </si>
   <si>
-    <t>10,800.00</t>
-  </si>
-  <si>
     <t>70800</t>
   </si>
   <si>
     <t>14750</t>
   </si>
   <si>
-    <t>4,500.00</t>
-  </si>
-  <si>
     <t>127,500.00</t>
   </si>
   <si>
@@ -4864,9 +4860,6 @@
     <t>150,450.00</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
     <t>1753400586</t>
   </si>
   <si>
@@ -4927,18 +4920,9 @@
     <t>1753_AutomationUSer</t>
   </si>
   <si>
-    <t>03/31/2021</t>
-  </si>
-  <si>
     <t>175310040</t>
   </si>
   <si>
-    <t>06AAECH8669K5</t>
-  </si>
-  <si>
-    <t>FN50113XCDNJX</t>
-  </si>
-  <si>
     <t>Invoice Specific Address</t>
   </si>
   <si>
@@ -4958,6 +4942,136 @@
   </si>
   <si>
     <t>Zip Code</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>06AAECH8669K51</t>
+  </si>
+  <si>
+    <t>FN50113XCDNJX2</t>
+  </si>
+  <si>
+    <t>110616</t>
+  </si>
+  <si>
+    <t>1753_AutoClient 30March2021 09:06:21</t>
+  </si>
+  <si>
+    <t>110616001</t>
+  </si>
+  <si>
+    <t>AutoGlobalBrand 30March2021 09:06:21</t>
+  </si>
+  <si>
+    <t>110616001001</t>
+  </si>
+  <si>
+    <t>AutoGlobalProduct 30March2021 09:06:21</t>
+  </si>
+  <si>
+    <t>126689</t>
+  </si>
+  <si>
+    <t>Global Vendor Name</t>
+  </si>
+  <si>
+    <t>GlobalVendor 30March2021 09:51:27</t>
+  </si>
+  <si>
+    <t>1,125.00</t>
+  </si>
+  <si>
+    <t>1753101715</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\Print Job Quote-9.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\Print Job Order Confirmation-4.pdf</t>
+  </si>
+  <si>
+    <t>1753100677</t>
+  </si>
+  <si>
+    <t>03/30/2021</t>
+  </si>
+  <si>
+    <t>14,750.00</t>
+  </si>
+  <si>
+    <t>1753103737</t>
+  </si>
+  <si>
+    <t>4/29/2021</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1753700557</t>
+  </si>
+  <si>
+    <t>AUTOFILL</t>
+  </si>
+  <si>
+    <t>175310039</t>
+  </si>
+  <si>
+    <t>HSN Code: 998314</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\Print Invoice Editing-8.pdf</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\P_JobInvoice-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1753400603
+</t>
+  </si>
+  <si>
+    <t>1753103744</t>
+  </si>
+  <si>
+    <t>1753400603</t>
+  </si>
+  <si>
+    <t>2001512578</t>
+  </si>
+  <si>
+    <t>1753101716</t>
+  </si>
+  <si>
+    <t>1753400604</t>
+  </si>
+  <si>
+    <t>1753103746</t>
+  </si>
+  <si>
+    <t>1753400602</t>
+  </si>
+  <si>
+    <t>1753101714</t>
+  </si>
+  <si>
+    <t>1753103747</t>
+  </si>
+  <si>
+    <t>1753103748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fields </t>
+  </si>
+  <si>
+    <t>ClientNumber</t>
+  </si>
+  <si>
+    <t>Collection Date</t>
+  </si>
+  <si>
+    <t>Payment_Mode</t>
   </si>
 </sst>
 </file>
@@ -6497,7 +6611,7 @@
       </c>
       <c r="G4" s="134"/>
       <c r="H4" s="132" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="I4" s="134" t="s">
         <v>840</v>
@@ -6513,7 +6627,7 @@
         <v>226</v>
       </c>
       <c r="O4" s="132" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="P4" s="134" t="s">
         <v>841</v>
@@ -6668,7 +6782,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,9 +6806,7 @@
       <c r="A2" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="134" t="s">
-        <v>1533</v>
-      </c>
+      <c r="C2" s="134"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
@@ -7738,6 +7850,60 @@
 
 <file path=xl/worksheets/sheet113.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D1" s="130" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="132">
+        <v>1284</v>
+      </c>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="132">
+        <v>1753</v>
+      </c>
+      <c r="B3" s="132">
+        <v>1753101716</v>
+      </c>
+      <c r="C3" s="132">
+        <v>1753400604</v>
+      </c>
+      <c r="D3" s="134" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8074,7 +8240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -8146,7 +8312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV3"/>
   <sheetViews>
@@ -8465,19 +8631,19 @@
         <v>1539</v>
       </c>
       <c r="F3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="G3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="H3" t="s">
+        <v>1561</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1561</v>
+      </c>
+      <c r="J3" t="s">
         <v>1540</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1148</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1541</v>
       </c>
       <c r="K3" t="s">
         <v>1282</v>
@@ -8492,19 +8658,19 @@
         <v>1290</v>
       </c>
       <c r="O3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="P3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="Q3" t="s">
-        <v>1291</v>
+        <v>1604</v>
       </c>
       <c r="R3" t="s">
-        <v>1148</v>
+        <v>1604</v>
       </c>
       <c r="S3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="T3" t="s">
         <v>1535</v>
@@ -8519,16 +8685,16 @@
         <v>1420</v>
       </c>
       <c r="X3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="Y3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="Z3" t="s">
-        <v>1543</v>
+        <v>1291</v>
       </c>
       <c r="AA3" t="s">
-        <v>1148</v>
+        <v>1291</v>
       </c>
       <c r="AB3" t="s">
         <v>1421</v>
@@ -8564,7 +8730,7 @@
         <v>177</v>
       </c>
       <c r="AV3" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
   </sheetData>
@@ -8573,7 +8739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG3"/>
   <sheetViews>
@@ -8985,19 +9151,19 @@
         <v>1539</v>
       </c>
       <c r="O3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="P3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="Q3" t="s">
-        <v>1540</v>
+        <v>1561</v>
       </c>
       <c r="R3" t="s">
-        <v>1148</v>
+        <v>1561</v>
       </c>
       <c r="S3" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="T3" t="s">
         <v>1282</v>
@@ -9012,73 +9178,73 @@
         <v>1290</v>
       </c>
       <c r="X3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="Y3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1604</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1604</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1559</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>1617</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AF3" t="s">
         <v>1138</v>
       </c>
-      <c r="Z3" t="s">
-        <v>1291</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>1148</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>1561</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>1535</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>1223</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>1419</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>1420</v>
-      </c>
       <c r="AG3" t="s">
-        <v>1149</v>
+        <v>1138</v>
       </c>
       <c r="AH3" t="s">
         <v>1138</v>
       </c>
       <c r="AI3" t="s">
-        <v>1543</v>
+        <v>1148</v>
       </c>
       <c r="AJ3" t="s">
         <v>1148</v>
       </c>
       <c r="AK3" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="AL3" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="AM3" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="AN3" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="AO3" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="AP3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="AQ3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="AR3" t="s">
-        <v>1563</v>
+        <v>1291</v>
       </c>
       <c r="AS3" t="s">
-        <v>1148</v>
+        <v>1291</v>
       </c>
       <c r="AT3" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="AU3" t="s">
         <v>1537</v>
@@ -9093,28 +9259,28 @@
         <v>1423</v>
       </c>
       <c r="AY3" t="s">
-        <v>1149</v>
+        <v>1412</v>
       </c>
       <c r="AZ3" t="s">
-        <v>1138</v>
+        <v>1413</v>
       </c>
       <c r="BA3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>1562</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="BG3" t="s">
         <v>1563</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>1148</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>1564</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>1544</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>1566</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>1565</v>
       </c>
     </row>
   </sheetData>
@@ -9123,7 +9289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -9170,7 +9336,7 @@
     </row>
     <row r="2" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="134" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>1068</v>
@@ -9182,7 +9348,7 @@
         <v>1070</v>
       </c>
       <c r="K2" s="134" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="132" customFormat="1" x14ac:dyDescent="0.25">
@@ -9210,7 +9376,7 @@
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
       <c r="K4" s="134" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>
@@ -9218,7 +9384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -9255,69 +9421,6 @@
       <c r="B3" s="130"/>
       <c r="C3" s="130">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="113" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1353</v>
       </c>
     </row>
   </sheetData>
@@ -9503,6 +9606,69 @@
 <file path=xl/worksheets/sheet120.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
@@ -9556,7 +9722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -9613,7 +9779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
@@ -9696,7 +9862,7 @@
         <v>1300</v>
       </c>
       <c r="E5" s="126" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -9767,7 +9933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -9844,7 +10010,7 @@
         <v>1431</v>
       </c>
       <c r="D6" s="126" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -9891,7 +10057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -9943,7 +10109,7 @@
         <v>1431</v>
       </c>
       <c r="C5" s="126" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -9981,7 +10147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -10031,7 +10197,7 @@
         <v>1431</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="D3" s="132"/>
       <c r="E3" s="132"/>
@@ -10103,7 +10269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -10167,7 +10333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -10222,7 +10388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -10274,100 +10440,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" style="132" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17" style="132" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" style="132" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.140625" style="132" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="132" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D1" s="57" t="s">
-        <v>1046</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>1047</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>1048</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="132" t="s">
-        <v>175</v>
-      </c>
-      <c r="I1" s="132" t="s">
-        <v>1273</v>
-      </c>
-      <c r="J1" s="132" t="s">
-        <v>1279</v>
-      </c>
-      <c r="K1" s="132" t="s">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="132">
-        <v>1707</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>1056</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>1053</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>1052</v>
-      </c>
-      <c r="I2" s="132" t="s">
-        <v>980</v>
-      </c>
-      <c r="J2" s="134" t="s">
-        <v>177</v>
-      </c>
-      <c r="K2" s="134" t="s">
-        <v>1380</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10830,6 +10902,100 @@
 
 <file path=xl/worksheets/sheet130.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" style="132" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" style="132" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" style="132" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" style="132" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" style="132" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" style="132" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" style="132" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.42578125" style="132" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.140625" style="132" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.28515625" style="132" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" style="132" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="132" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="132" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="132" t="s">
+        <v>1273</v>
+      </c>
+      <c r="J1" s="132" t="s">
+        <v>1279</v>
+      </c>
+      <c r="K1" s="132" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="132">
+        <v>1707</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I2" s="132" t="s">
+        <v>980</v>
+      </c>
+      <c r="J2" s="134" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="134" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10958,7 +11124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -11018,12 +11184,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="XEK1" workbookViewId="0">
-      <selection activeCell="XFD8" sqref="XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11070,7 +11236,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="97" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B1" s="122">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -11133,7 +11346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet136.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -11205,7 +11418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet137.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -11466,7 +11679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet136.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet138.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -11502,7 +11715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet137.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet139.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -11576,417 +11789,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet138.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="35">
-        <v>1707</v>
-      </c>
-      <c r="C1" s="35">
-        <v>1712</v>
-      </c>
-      <c r="D1" s="35">
-        <v>1753</v>
-      </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1329</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D2" s="132" t="s">
-        <v>1512</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1330</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D3" s="132" t="s">
-        <v>1513</v>
-      </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1331</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D4" s="132" t="s">
-        <v>1514</v>
-      </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1332</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D5" s="132" t="s">
-        <v>1515</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1333</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1104</v>
-      </c>
-      <c r="D6" s="132" t="s">
-        <v>1516</v>
-      </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1334</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D7" s="132" t="s">
-        <v>1517</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D8" s="132" t="s">
-        <v>1518</v>
-      </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D9" s="132" t="s">
-        <v>1519</v>
-      </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1337</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1116</v>
-      </c>
-      <c r="D10" s="132" t="s">
-        <v>1520</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1117</v>
-      </c>
-      <c r="D11" s="132" t="s">
-        <v>1521</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet139.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="90" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="87" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="87" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1351</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1352</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12372,6 +12174,417 @@
       </c>
       <c r="O3">
         <v>998312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet140.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="35">
+        <v>1707</v>
+      </c>
+      <c r="C1" s="35">
+        <v>1712</v>
+      </c>
+      <c r="D1" s="35">
+        <v>1753</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D2" s="132" t="s">
+        <v>1512</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D3" s="132" t="s">
+        <v>1513</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D4" s="132" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D5" s="132" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D6" s="132" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D7" s="132" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D10" s="132" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D11" s="132" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="87" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="87" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="87" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="88" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1352</v>
       </c>
     </row>
   </sheetData>
@@ -12778,7 +12991,7 @@
   <dimension ref="A1:BB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13067,6 +13280,9 @@
       <c r="A3">
         <v>1753</v>
       </c>
+      <c r="C3">
+        <v>17539905</v>
+      </c>
       <c r="D3" t="s">
         <v>1171</v>
       </c>
@@ -13092,7 +13308,7 @@
         <v>123</v>
       </c>
       <c r="L3" s="102" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
   </sheetData>
@@ -14232,25 +14448,26 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FM84"/>
+  <dimension ref="A1:FN85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.42578125" style="28" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="40" style="28" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40" style="130" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" style="130" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.140625" style="28" customWidth="1" collapsed="1"/>
-    <col min="7" max="169" width="32" style="28" customWidth="1" collapsed="1"/>
-    <col min="170" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="2" max="2" width="52.42578125" style="130" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40" style="28" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40" style="130" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.42578125" style="130" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.140625" style="28" customWidth="1" collapsed="1"/>
+    <col min="8" max="170" width="32" style="28" customWidth="1" collapsed="1"/>
+    <col min="171" max="16384" width="9.140625" style="28" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>157</v>
       </c>
@@ -14258,14 +14475,14 @@
         <v>1753</v>
       </c>
       <c r="C1" s="14"/>
-      <c r="D1" s="14">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14">
         <v>1707</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14">
         <v>1712</v>
       </c>
-      <c r="G1" s="14"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -14428,892 +14645,1064 @@
       <c r="FK1" s="14"/>
       <c r="FL1" s="14"/>
       <c r="FM1" s="14"/>
-    </row>
-    <row r="2" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="FN1" s="14"/>
+    </row>
+    <row r="2" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>1572</v>
+        <v>1624</v>
       </c>
       <c r="C2" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D2" t="s">
         <v>1533</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1489</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="F2" s="132" t="s">
         <v>1411</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="57"/>
       <c r="J2" s="57"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="56"/>
-    </row>
-    <row r="3" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="K2" s="57"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="56"/>
+    </row>
+    <row r="3" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>1588</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1546</v>
+      <c r="B3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>1584</v>
       </c>
       <c r="D3" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E3" t="s">
         <v>1460</v>
       </c>
-      <c r="E3" s="132"/>
-      <c r="F3" s="57"/>
-    </row>
-    <row r="4" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F3" s="132"/>
+      <c r="G3" s="57"/>
+    </row>
+    <row r="4" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>1558</v>
-      </c>
-      <c r="D4" s="28" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1556</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>1450</v>
       </c>
     </row>
-    <row r="5" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="C5" s="134"/>
-      <c r="D5" t="s">
+        <v>1608</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D5" s="134"/>
+      <c r="E5" t="s">
         <v>1435</v>
       </c>
-      <c r="E5" s="132"/>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="132"/>
+      <c r="G5" s="56" t="s">
         <v>1141</v>
       </c>
     </row>
-    <row r="6" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>684</v>
       </c>
-      <c r="B6" s="134" t="s">
-        <v>1552</v>
-      </c>
-      <c r="C6" s="132"/>
-      <c r="D6" t="s">
+      <c r="B6" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C6" s="134" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D6" s="132"/>
+      <c r="E6" t="s">
         <v>1439</v>
       </c>
-      <c r="E6" s="132"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F6" s="132"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>685</v>
       </c>
       <c r="B7" t="s">
-        <v>1551</v>
-      </c>
-      <c r="C7" s="132"/>
-      <c r="D7" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D7" s="132"/>
+      <c r="E7" t="s">
         <v>1432</v>
       </c>
-      <c r="E7" s="132"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F7" s="132"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>694</v>
       </c>
       <c r="B8" t="s">
-        <v>1557</v>
-      </c>
-      <c r="C8" s="132"/>
-      <c r="D8" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D8" s="132"/>
+      <c r="E8" t="s">
         <v>690</v>
       </c>
-      <c r="E8" s="132"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F8" s="132"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>695</v>
       </c>
       <c r="B9" t="s">
         <v>1516</v>
       </c>
-      <c r="C9" s="132"/>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D9" s="132"/>
+      <c r="E9" t="s">
         <v>1333</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F9" s="132"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>696</v>
       </c>
       <c r="B10" t="s">
-        <v>1555</v>
-      </c>
-      <c r="C10" s="132"/>
-      <c r="D10" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D10" s="132"/>
+      <c r="E10" t="s">
         <v>1448</v>
       </c>
-      <c r="E10" s="132"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="F10" s="132"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="12" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="13" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>752</v>
       </c>
-      <c r="B13" s="134" t="s">
+      <c r="B13" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C13" s="134" t="s">
         <v>1523</v>
       </c>
-      <c r="C13" s="134"/>
-      <c r="D13" t="s">
+      <c r="D13" s="134"/>
+      <c r="E13" t="s">
         <v>1402</v>
       </c>
-      <c r="E13" s="132"/>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="132"/>
+      <c r="G13" s="56" t="s">
         <v>1147</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="14" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>753</v>
       </c>
       <c r="B14" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C14" t="s">
         <v>1522</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" t="s">
+      <c r="D14" s="132"/>
+      <c r="E14" t="s">
         <v>1403</v>
       </c>
-      <c r="E14" s="132"/>
-      <c r="F14" t="s">
+      <c r="F14" s="132"/>
+      <c r="G14" t="s">
         <v>1142</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>990</v>
       </c>
     </row>
-    <row r="15" spans="1:169" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>754</v>
       </c>
-      <c r="B15" s="134" t="s">
+      <c r="B15" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C15" s="134" t="s">
         <v>1526</v>
       </c>
-      <c r="C15" s="134"/>
-      <c r="D15" t="s">
+      <c r="D15" s="134"/>
+      <c r="E15" t="s">
         <v>1404</v>
       </c>
-      <c r="E15" s="132"/>
-      <c r="F15" t="s">
-        <v>991</v>
-      </c>
+      <c r="F15" s="132"/>
       <c r="G15" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="16" spans="1:169" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:170" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>755</v>
       </c>
       <c r="B16" t="s">
+        <v>1598</v>
+      </c>
+      <c r="C16" t="s">
         <v>1525</v>
       </c>
-      <c r="C16" s="132"/>
-      <c r="D16" t="s">
+      <c r="D16" s="132"/>
+      <c r="E16" t="s">
         <v>1405</v>
       </c>
-      <c r="E16" s="132"/>
-      <c r="F16" t="s">
-        <v>992</v>
-      </c>
+      <c r="F16" s="132"/>
       <c r="G16" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>756</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>1524</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>1406</v>
       </c>
-      <c r="E17" s="132"/>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="132"/>
+      <c r="G17" s="28" t="s">
         <v>1146</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="H17" s="28" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>757</v>
       </c>
       <c r="B18" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C18" t="s">
         <v>1527</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" t="s">
+      <c r="D18" s="132"/>
+      <c r="E18" t="s">
         <v>1407</v>
       </c>
-      <c r="E18" s="132"/>
-      <c r="F18" t="s">
-        <v>993</v>
-      </c>
+      <c r="F18" s="132"/>
       <c r="G18" t="s">
         <v>993</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C21" s="57" t="s">
         <v>1528</v>
       </c>
-      <c r="C21" s="57"/>
-      <c r="D21" t="s">
+      <c r="D21" s="57"/>
+      <c r="E21" t="s">
         <v>1409</v>
       </c>
-      <c r="E21" s="132"/>
-      <c r="F21" s="57"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="132"/>
+      <c r="G21" s="57"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>825</v>
       </c>
-      <c r="B22"/>
-      <c r="C22" s="132"/>
-      <c r="D22"/>
-      <c r="E22" s="132"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22"/>
+      <c r="D22" s="132"/>
+      <c r="E22"/>
+      <c r="F22" s="132"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>842</v>
       </c>
       <c r="B23" t="s">
-        <v>1580</v>
-      </c>
-      <c r="C23" s="132"/>
-      <c r="D23" t="s">
+        <v>1630</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D23" s="132"/>
+      <c r="E23" t="s">
         <v>1451</v>
       </c>
-      <c r="E23" s="132"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" s="132"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D24"/>
-      <c r="E24" s="132"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+      <c r="F24" s="132"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>848</v>
       </c>
       <c r="B25" t="s">
-        <v>1572</v>
-      </c>
-      <c r="C25" s="134"/>
-      <c r="D25" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D25" s="134"/>
+      <c r="E25" t="s">
         <v>1489</v>
       </c>
-      <c r="E25" s="132"/>
-      <c r="F25" s="56" t="s">
+      <c r="F25" s="132"/>
+      <c r="G25" s="56" t="s">
         <v>1143</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>849</v>
       </c>
       <c r="B26" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="132"/>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
         <v>177</v>
       </c>
-      <c r="E26" s="132"/>
-      <c r="F26" t="s">
+      <c r="D26" s="132"/>
+      <c r="E26" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="132"/>
+      <c r="G26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1000</v>
       </c>
-      <c r="B27"/>
-      <c r="C27" s="132"/>
-      <c r="D27"/>
-      <c r="E27" s="132"/>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="132"/>
+      <c r="C27"/>
+      <c r="D27" s="132"/>
+      <c r="E27"/>
+      <c r="F27" s="132"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1012</v>
       </c>
-      <c r="B28" s="134" t="s">
-        <v>1553</v>
-      </c>
-      <c r="C28" s="134"/>
-      <c r="D28" t="s">
+      <c r="B28" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C28" s="134" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D28" s="134"/>
+      <c r="E28" t="s">
         <v>1440</v>
       </c>
-      <c r="E28" s="132"/>
-      <c r="F28" s="102" t="s">
+      <c r="F28" s="132"/>
+      <c r="G28" s="102" t="s">
         <v>1144</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1035</v>
       </c>
       <c r="B29" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C29" t="s">
         <v>985</v>
       </c>
-      <c r="C29" s="132"/>
-      <c r="D29" t="s">
+      <c r="D29" s="132"/>
+      <c r="E29" t="s">
         <v>985</v>
       </c>
-      <c r="E29" s="132" t="s">
+      <c r="F29" s="132" t="s">
         <v>1061</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>835</v>
       </c>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="132"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1037</v>
       </c>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="132"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1038</v>
       </c>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="132"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1063</v>
       </c>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="132"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1064</v>
       </c>
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="132"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1039</v>
       </c>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="132"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1065</v>
       </c>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="132"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1042</v>
       </c>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="132"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1043</v>
       </c>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="132"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1066</v>
       </c>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="132"/>
+      <c r="G39"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1067</v>
       </c>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="132"/>
+      <c r="G40"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>1089</v>
       </c>
-      <c r="B41" s="134" t="s">
+      <c r="B41" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C41" s="134" t="s">
         <v>1533</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>1411</v>
       </c>
-      <c r="E41" s="132"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="132"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1139</v>
       </c>
-      <c r="D42"/>
-      <c r="E42" s="132"/>
-      <c r="F42" t="s">
+      <c r="B42" s="132"/>
+      <c r="E42"/>
+      <c r="F42" s="132"/>
+      <c r="G42" t="s">
         <v>1150</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1266</v>
       </c>
-      <c r="D43"/>
-      <c r="E43" s="132"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="132"/>
+      <c r="E43"/>
+      <c r="F43" s="132"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>1267</v>
       </c>
-      <c r="D44"/>
-      <c r="E44" s="132"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44"/>
+      <c r="F44" s="132"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>1268</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>1269</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>1270</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>1271</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1303</v>
       </c>
-      <c r="D50"/>
-      <c r="E50" s="132"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="132"/>
+      <c r="E50"/>
+      <c r="F50" s="132"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1304</v>
       </c>
-      <c r="D51"/>
-      <c r="E51" s="132"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="132"/>
+      <c r="E51"/>
+      <c r="F51" s="132"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1354</v>
       </c>
-      <c r="D52"/>
-      <c r="E52" s="132"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="132"/>
+      <c r="E52"/>
+      <c r="F52" s="132"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1356</v>
       </c>
-      <c r="D53"/>
-      <c r="E53" s="132"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="132"/>
+      <c r="E53"/>
+      <c r="F53" s="132"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1228</v>
       </c>
-      <c r="D54"/>
-      <c r="E54" s="132"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="132"/>
+      <c r="E54"/>
+      <c r="F54" s="132"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1357</v>
       </c>
-      <c r="D55"/>
-      <c r="E55" s="132"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="132"/>
+      <c r="E55"/>
+      <c r="F55" s="132"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1358</v>
       </c>
-      <c r="D56"/>
-      <c r="E56" s="132"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="132"/>
+      <c r="E56"/>
+      <c r="F56" s="132"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
       <c r="B57" t="s">
-        <v>1559</v>
-      </c>
-      <c r="D57" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1557</v>
+      </c>
+      <c r="E57" t="s">
         <v>1441</v>
       </c>
-      <c r="E57" s="132"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="132"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>1379</v>
       </c>
-      <c r="D58" t="s">
+      <c r="B58" s="132"/>
+      <c r="E58" t="s">
         <v>1459</v>
       </c>
-      <c r="E58" s="132"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="132"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1408</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" t="s">
         <v>235</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C59" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E59" s="132"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>235</v>
+      </c>
+      <c r="F59" s="132"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1410</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B60" t="s">
         <v>235</v>
       </c>
-      <c r="D60" t="s">
+      <c r="C60" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E60" s="132"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>235</v>
+      </c>
+      <c r="F60" s="132"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1429</v>
       </c>
       <c r="B61" t="s">
-        <v>1545</v>
-      </c>
-      <c r="C61" s="132"/>
-      <c r="D61" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D61" s="132"/>
+      <c r="E61" t="s">
         <v>1490</v>
       </c>
-      <c r="E61" s="132"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="132"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1430</v>
       </c>
       <c r="B62" t="s">
-        <v>1545</v>
-      </c>
-      <c r="D62" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E62" t="s">
         <v>1491</v>
       </c>
-      <c r="E62" s="132"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="132"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>1436</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="B63" t="s">
         <v>1237</v>
       </c>
-      <c r="D63" t="s">
+      <c r="C63" s="28" t="s">
         <v>1237</v>
       </c>
-      <c r="E63" s="132"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F63" s="132"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1437</v>
       </c>
-      <c r="B64" s="28" t="s">
-        <v>1554</v>
-      </c>
-      <c r="D64" s="120" t="s">
+      <c r="B64" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>1552</v>
+      </c>
+      <c r="E64" s="120" t="s">
         <v>1445</v>
       </c>
-      <c r="E64" s="120"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="120"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1438</v>
       </c>
-      <c r="B65" s="57" t="s">
+      <c r="B65" t="s">
         <v>1290</v>
       </c>
-      <c r="D65" s="134" t="s">
+      <c r="C65" s="57" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E65" s="134" t="s">
         <v>1446</v>
       </c>
-      <c r="E65" s="134"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="134"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1447</v>
       </c>
       <c r="B66" t="s">
-        <v>1552</v>
-      </c>
-      <c r="D66" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E66" t="s">
         <v>1439</v>
       </c>
-      <c r="E66" s="132"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="132"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1452</v>
       </c>
       <c r="B67" t="s">
-        <v>1581</v>
-      </c>
-      <c r="D67" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E67" t="s">
         <v>1453</v>
       </c>
-      <c r="E67" s="132"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="132"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1454</v>
       </c>
       <c r="B68" t="s">
         <v>1235</v>
       </c>
-      <c r="D68" t="s">
+      <c r="C68" t="s">
         <v>1235</v>
       </c>
-      <c r="E68" s="132"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F68" s="132"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1455</v>
       </c>
       <c r="B69" t="s">
-        <v>1582</v>
-      </c>
-      <c r="D69" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E69" t="s">
         <v>1456</v>
       </c>
-      <c r="E69" s="132"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="132"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1457</v>
       </c>
       <c r="B70" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D70" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1580</v>
+      </c>
+      <c r="E70" t="s">
         <v>1458</v>
       </c>
-      <c r="E70" s="132"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="132"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1470</v>
       </c>
       <c r="B71" t="s">
-        <v>1545</v>
-      </c>
-      <c r="D71" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E71" t="s">
         <v>1471</v>
       </c>
-      <c r="E71" s="132"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="132"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1472</v>
       </c>
       <c r="B72" t="s">
-        <v>1545</v>
-      </c>
-      <c r="D72" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E72" t="s">
         <v>1473</v>
       </c>
-      <c r="E72" s="132"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="132"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1474</v>
       </c>
-      <c r="B73" s="28" t="s">
-        <v>1567</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="B73" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>1564</v>
+      </c>
+      <c r="E73" t="s">
         <v>1475</v>
       </c>
-      <c r="E73" s="132"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="132"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1476</v>
       </c>
       <c r="B74" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D74" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1566</v>
+      </c>
+      <c r="E74" t="s">
         <v>1477</v>
       </c>
-      <c r="E74" s="132"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="132"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1478</v>
       </c>
       <c r="B75" t="s">
-        <v>1567</v>
-      </c>
-      <c r="D75" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1564</v>
+      </c>
+      <c r="E75" t="s">
         <v>1479</v>
       </c>
-      <c r="E75" s="132"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="132"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1480</v>
       </c>
       <c r="B76" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C76" t="s">
         <v>1533</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>1411</v>
       </c>
-      <c r="E76" s="132"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="132"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>1483</v>
       </c>
-      <c r="D77" s="28" t="s">
+      <c r="E77" s="28" t="s">
         <v>1482</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>1484</v>
       </c>
-      <c r="D78" s="28" t="s">
+      <c r="E78" s="28" t="s">
         <v>1481</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1485</v>
       </c>
       <c r="B79" t="s">
-        <v>1571</v>
-      </c>
-      <c r="D79" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E79" t="s">
         <v>1486</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1487</v>
       </c>
       <c r="B80" t="s">
-        <v>1570</v>
-      </c>
-      <c r="D80" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E80" t="s">
         <v>1482</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1488</v>
       </c>
       <c r="B81" t="s">
-        <v>1546</v>
-      </c>
-      <c r="D81" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1544</v>
+      </c>
+      <c r="E81" t="s">
         <v>1481</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1493</v>
       </c>
       <c r="B82" t="s">
-        <v>1576</v>
-      </c>
-      <c r="D82" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1573</v>
+      </c>
+      <c r="E82" t="s">
         <v>1494</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1495</v>
       </c>
       <c r="B83" t="s">
-        <v>1575</v>
-      </c>
-      <c r="D83" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1572</v>
+      </c>
+      <c r="E83" t="s">
         <v>1492</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1496</v>
       </c>
       <c r="B84" t="s">
-        <v>1572</v>
-      </c>
-      <c r="D84" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E84" t="s">
         <v>1489</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1603</v>
       </c>
     </row>
   </sheetData>
@@ -15330,7 +15719,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15365,8 +15754,8 @@
       <c r="B3" s="28" t="s">
         <v>1448</v>
       </c>
-      <c r="C3" s="130" t="s">
-        <v>1555</v>
+      <c r="C3" s="57" t="s">
+        <v>1613</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15541,7 +15930,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15583,7 +15972,7 @@
         <v>686</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -15664,7 +16053,7 @@
         <v>1431</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>1579</v>
+        <v>1615</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -15697,7 +16086,7 @@
         <v>697</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -15979,7 +16368,7 @@
         <v>1378</v>
       </c>
       <c r="D2" s="130" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -16042,8 +16431,8 @@
       <c r="C7" s="15" t="s">
         <v>1431</v>
       </c>
-      <c r="D7" s="75" t="s">
-        <v>1579</v>
+      <c r="D7" s="77" t="s">
+        <v>1615</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -16056,8 +16445,8 @@
       <c r="C8" s="15" t="s">
         <v>1442</v>
       </c>
-      <c r="D8" s="75" t="s">
-        <v>1587</v>
+      <c r="D8" s="77" t="s">
+        <v>1615</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -16088,7 +16477,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16126,7 +16515,7 @@
         <v>686</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -16214,8 +16603,8 @@
       <c r="B7" s="18" t="s">
         <v>1431</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>1431</v>
+      <c r="C7" s="77" t="s">
+        <v>1615</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -16251,7 +16640,7 @@
         <v>697</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -16520,8 +16909,8 @@
       <c r="B24" s="16" t="s">
         <v>687</v>
       </c>
-      <c r="C24" s="75" t="s">
-        <v>1579</v>
+      <c r="C24" s="77" t="s">
+        <v>1615</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -16538,8 +16927,8 @@
       <c r="B25" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="C25" s="75" t="s">
-        <v>1587</v>
+      <c r="C25" s="77" t="s">
+        <v>1615</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -18575,7 +18964,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23195,7 +23584,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23268,7 +23657,7 @@
         <v>1431</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>1547</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -23279,7 +23668,7 @@
         <v>10000</v>
       </c>
       <c r="C7" s="130" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -23391,7 +23780,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23686,7 +24075,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23746,16 +24135,16 @@
         <v>1753</v>
       </c>
       <c r="C3" s="134" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D3" s="134" t="s">
+        <v>1609</v>
+      </c>
+      <c r="E3" s="134" t="s">
+        <v>1546</v>
+      </c>
+      <c r="F3" s="134" t="s">
         <v>1547</v>
-      </c>
-      <c r="D3" s="134" t="s">
-        <v>1547</v>
-      </c>
-      <c r="E3" s="134" t="s">
-        <v>1548</v>
-      </c>
-      <c r="F3" s="134" t="s">
-        <v>1549</v>
       </c>
       <c r="G3" s="134" t="s">
         <v>1434</v>
@@ -23857,8 +24246,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24066,7 +24455,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>985</v>
+        <v>1061</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>985</v>
@@ -24086,7 +24475,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>986</v>
+        <v>1062</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>986</v>
@@ -24466,10 +24855,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24478,27 +24867,30 @@
     <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2">
         <v>1707</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="56"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>227</v>
       </c>
@@ -25154,7 +25546,7 @@
         <v>1481</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>1546</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -25165,7 +25557,7 @@
         <v>1182</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -25192,7 +25584,7 @@
         <v>1482</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>1570</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -25263,7 +25655,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25292,7 +25684,7 @@
         <v>1489</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>1572</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -25330,7 +25722,7 @@
         <v>1492</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>1575</v>
+        <v>1627</v>
       </c>
     </row>
   </sheetData>
@@ -25495,8 +25887,8 @@
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A12" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25602,7 +25994,7 @@
         <v>1399</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>1589</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -25613,7 +26005,7 @@
         <v>1400</v>
       </c>
       <c r="C10" s="134" t="s">
-        <v>1590</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -25810,46 +26202,46 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="132" t="s">
-        <v>1591</v>
+        <v>1585</v>
       </c>
       <c r="B29" s="132" t="s">
-        <v>1592</v>
+        <v>1586</v>
       </c>
       <c r="C29" s="132" t="s">
-        <v>1592</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="132" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
       <c r="B30" s="132" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
       <c r="C30" s="132" t="s">
-        <v>1594</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="132" t="s">
-        <v>1595</v>
+        <v>1589</v>
       </c>
       <c r="B31" s="132" t="s">
-        <v>1596</v>
+        <v>1590</v>
       </c>
       <c r="C31" s="132" t="s">
-        <v>1596</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="132" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
       <c r="B32" s="134" t="s">
-        <v>723</v>
+        <v>1592</v>
       </c>
       <c r="C32" s="134" t="s">
-        <v>723</v>
+        <v>1592</v>
       </c>
     </row>
   </sheetData>
@@ -25870,7 +26262,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Purchaser order MPL
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_IND_REGRESSION.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="130" activeTab="133"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="137" activeTab="139"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -151,12 +151,13 @@
     <sheet name="Modify budget" sheetId="138" r:id="rId137"/>
     <sheet name="Copy budget" sheetId="139" r:id="rId138"/>
     <sheet name="ExpensesMPL" sheetId="140" r:id="rId139"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId140"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId141"/>
+    <sheet name="PurchaseOrderMPL" sheetId="153" r:id="rId140"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId141"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId142"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -164,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4690" uniqueCount="1635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4722" uniqueCount="1646">
   <si>
     <t>Description</t>
   </si>
@@ -4992,9 +4993,6 @@
     <t>C:\GlobalTestAutomation2\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\Print Job Order Confirmation-4.pdf</t>
   </si>
   <si>
-    <t>1753100677</t>
-  </si>
-  <si>
     <t>03/30/2021</t>
   </si>
   <si>
@@ -5072,12 +5070,50 @@
   </si>
   <si>
     <t>Payment_Mode</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>PurchaseOrderMPL</t>
+  </si>
+  <si>
+    <t>1753101528</t>
+  </si>
+  <si>
+    <t>Towards the cost of following Image Purchased for Client Volvo:
+552552059 (The Image Bank) Mumbai, Victoria Terminus railways station Royalty-free image</t>
+  </si>
+  <si>
+    <t>14,030.00</t>
+  </si>
+  <si>
+    <t>Photographer: Tuul &amp; Bruno Morandi Description: Mumbai, Victoria Terminus railways station Product type: Royalty-free image File Size/DPI: 103.4 MB - 7360 x 4912 px (62.31 x 41.59 cm) - 300 dpi - RGB</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\P_PurchaseOrder-6.pdf</t>
+  </si>
+  <si>
+    <t>1753100612</t>
+  </si>
+  <si>
+    <t>1284200514</t>
+  </si>
+  <si>
+    <t>平面修片-3rd</t>
+  </si>
+  <si>
+    <t>4,000.00</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuiteAutomation\WppRegPack\MPLReports\Critical_Regression\India\1753\P_PurchaseOrder-7.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5900,9 +5936,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6002,9 +6038,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6224,8 +6260,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6260,8 +6296,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6305,17 +6341,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -6463,17 +6499,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -6652,7 +6688,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6692,15 +6728,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6787,8 +6823,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="17.85546875" collapsed="true"/>
+    <col min="2" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6835,13 +6871,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6932,16 +6968,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7072,7 +7108,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7290,9 +7326,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7541,44 +7577,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="15" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -7812,9 +7848,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7858,7 +7894,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7899,6 +7935,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7912,51 +7949,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="15" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" x14ac:dyDescent="0.25">
@@ -8250,13 +8287,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="132" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="132" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" style="132" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="132" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" style="132" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="132" width="17.85546875" collapsed="true"/>
+    <col min="7" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8309,6 +8346,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9193,7 +9231,7 @@
         <v>1559</v>
       </c>
       <c r="AC3" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="AD3" t="s">
         <v>1148</v>
@@ -9381,6 +9419,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9442,10 +9481,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="46" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" style="46" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="46" width="30.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="46" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="28" width="26.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -9616,8 +9655,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9679,8 +9718,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9735,9 +9774,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="11.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9789,10 +9828,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23" style="99" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" style="99" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" style="99" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="8.7109375" style="99" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" style="99" width="23.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="99" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="99" width="22.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="99" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -9943,10 +9982,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="99" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" style="99" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.140625" style="99" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="8.7109375" style="99" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="99" width="22.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="99" width="29.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="99" width="34.140625" collapsed="true"/>
+    <col min="4" max="16384" style="99" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -10067,9 +10106,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="99" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" style="99" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7109375" style="99" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="99" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="99" width="22.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="99" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -10157,9 +10196,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="131" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" style="131" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7109375" style="131" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="131" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="131" width="16.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="131" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -10279,9 +10318,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="99" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" style="99" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7109375" style="99" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="99" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="99" width="16.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="99" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10343,9 +10382,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="131" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" style="131" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7109375" style="131" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="131" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="131" width="16.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="131" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10398,9 +10437,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="131" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.28515625" style="131" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="8.7109375" style="131" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="131" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="131" width="16.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="131" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10456,40 +10495,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="56" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
@@ -10910,18 +10949,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" style="132" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17" style="132" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" style="132" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.140625" style="132" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="22.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="20.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="132" width="17.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="132" width="16.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="132" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="132" width="17.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="132" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="132" width="20.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="132" width="17.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="132" width="15.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="132" width="13.42578125" collapsed="true"/>
+    <col min="12" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -11004,20 +11043,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="21.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="23.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="32.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="132" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="132" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="132" width="23.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="132" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="132" width="19.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="132" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="132" width="21.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="132" width="23.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="132" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="132" width="18.85546875" collapsed="true"/>
+    <col min="14" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -11134,8 +11173,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11194,8 +11233,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11240,18 +11279,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="97" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B1" s="122">
         <v>1753</v>
@@ -11259,20 +11298,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B3" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B4" t="s">
         <v>1235</v>
@@ -11280,6 +11319,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11296,8 +11336,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="18.0" collapsed="true"/>
+    <col min="2" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11359,9 +11399,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="21.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="130" width="26.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11431,16 +11471,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="132" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="9.140625" style="132" collapsed="1"/>
-    <col min="8" max="8" width="12" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="132" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" style="132" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="12.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="132" width="20.85546875" collapsed="true"/>
+    <col min="5" max="7" style="132" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="132" width="12.0" collapsed="true"/>
+    <col min="9" max="9" style="132" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="132" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="132" width="11.0" collapsed="true"/>
+    <col min="12" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
@@ -11692,8 +11732,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" style="130" width="11.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11723,15 +11763,15 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="132" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" style="132" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="11.7109375" collapsed="true"/>
+    <col min="4" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -11805,41 +11845,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -12183,6 +12223,106 @@
 </file>
 
 <file path=xl/worksheets/sheet140.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="130" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C1" s="130" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="132" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="130" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="132" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="130" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H1" s="130" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="132" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="130" t="s">
+        <v>170</v>
+      </c>
+      <c r="K1" s="132" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="130" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="132">
+        <v>1753</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1639</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1634</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -12195,11 +12335,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="132" width="27.5703125" collapsed="true"/>
+    <col min="5" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -12450,7 +12590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet141.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet142.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -12463,8 +12603,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12606,41 +12746,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -12996,48 +13136,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.25">
@@ -13330,41 +13470,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -13720,41 +13860,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -14110,41 +14250,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="58" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="57" max="58" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.25">
@@ -14448,23 +14588,23 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:FN85"/>
+  <dimension ref="A1:FN86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" style="28" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.42578125" style="130" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40" style="28" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40" style="130" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.42578125" style="130" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.140625" style="28" customWidth="1" collapsed="1"/>
-    <col min="8" max="170" width="32" style="28" customWidth="1" collapsed="1"/>
-    <col min="171" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="28" width="52.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="130" width="52.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="28" width="40.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="130" width="40.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="28" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="130" width="36.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="28" width="36.140625" collapsed="true"/>
+    <col min="8" max="170" customWidth="true" style="28" width="32.0" collapsed="true"/>
+    <col min="171" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:170" x14ac:dyDescent="0.25">
@@ -14652,7 +14792,7 @@
         <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C2" t="s">
         <v>1569</v>
@@ -14679,7 +14819,7 @@
         <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>1584</v>
@@ -14698,7 +14838,7 @@
         <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C4" t="s">
         <v>1556</v>
@@ -14711,8 +14851,8 @@
       <c r="A5" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="B5" t="s">
-        <v>1608</v>
+      <c r="B5" s="134" t="s">
+        <v>1641</v>
       </c>
       <c r="C5" t="s">
         <v>1548</v>
@@ -14731,7 +14871,7 @@
         <v>684</v>
       </c>
       <c r="B6" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C6" s="134" t="s">
         <v>1550</v>
@@ -14799,7 +14939,7 @@
         <v>696</v>
       </c>
       <c r="B10" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C10" t="s">
         <v>1553</v>
@@ -14994,7 +15134,7 @@
         <v>842</v>
       </c>
       <c r="B23" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="C23" t="s">
         <v>1577</v>
@@ -15018,7 +15158,7 @@
         <v>848</v>
       </c>
       <c r="B25" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C25" t="s">
         <v>1569</v>
@@ -15067,7 +15207,7 @@
         <v>1012</v>
       </c>
       <c r="B28" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C28" s="134" t="s">
         <v>1551</v>
@@ -15407,7 +15547,7 @@
         <v>1437</v>
       </c>
       <c r="B64" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C64" s="28" t="s">
         <v>1552</v>
@@ -15437,7 +15577,7 @@
         <v>1447</v>
       </c>
       <c r="B66" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C66" t="s">
         <v>1550</v>
@@ -15482,7 +15622,7 @@
         <v>1455</v>
       </c>
       <c r="B69" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="C69" t="s">
         <v>1579</v>
@@ -15512,7 +15652,7 @@
         <v>1470</v>
       </c>
       <c r="B71" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C71" t="s">
         <v>1543</v>
@@ -15527,7 +15667,7 @@
         <v>1472</v>
       </c>
       <c r="B72" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C72" t="s">
         <v>1543</v>
@@ -15542,7 +15682,7 @@
         <v>1474</v>
       </c>
       <c r="B73" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C73" s="28" t="s">
         <v>1564</v>
@@ -15557,7 +15697,7 @@
         <v>1476</v>
       </c>
       <c r="B74" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C74" t="s">
         <v>1566</v>
@@ -15572,7 +15712,7 @@
         <v>1478</v>
       </c>
       <c r="B75" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="C75" t="s">
         <v>1564</v>
@@ -15618,7 +15758,7 @@
         <v>1485</v>
       </c>
       <c r="B79" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="C79" t="s">
         <v>1568</v>
@@ -15632,7 +15772,7 @@
         <v>1487</v>
       </c>
       <c r="B80" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="C80" t="s">
         <v>1567</v>
@@ -15646,7 +15786,7 @@
         <v>1488</v>
       </c>
       <c r="B81" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="C81" t="s">
         <v>1544</v>
@@ -15660,7 +15800,7 @@
         <v>1493</v>
       </c>
       <c r="B82" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C82" t="s">
         <v>1573</v>
@@ -15674,7 +15814,7 @@
         <v>1495</v>
       </c>
       <c r="B83" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="C83" t="s">
         <v>1572</v>
@@ -15688,7 +15828,7 @@
         <v>1496</v>
       </c>
       <c r="B84" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="C84" t="s">
         <v>1569</v>
@@ -15703,6 +15843,14 @@
       </c>
       <c r="B85" t="s">
         <v>1603</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1645</v>
       </c>
     </row>
   </sheetData>
@@ -15724,9 +15872,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19" style="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="130" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15755,7 +15903,7 @@
         <v>1448</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15935,16 +16083,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.140625" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="60.140625" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="51" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="58.140625" style="28" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="57.7109375" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="63.7109375" style="28" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="45.28515625" style="28" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="28" width="31.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="60.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="130" width="60.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="28" width="51.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="28" width="51.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="28" width="58.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="28" width="57.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="28" width="63.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="28" width="45.28515625" collapsed="true"/>
+    <col min="10" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16053,7 +16201,7 @@
         <v>1431</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -16336,11 +16484,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.140625" style="28" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.5703125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.5703125" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="28" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="28" width="23.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="28" width="31.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="130" width="31.5703125" collapsed="true"/>
+    <col min="5" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16432,7 +16580,7 @@
         <v>1431</v>
       </c>
       <c r="D7" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -16446,7 +16594,7 @@
         <v>1442</v>
       </c>
       <c r="D8" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -16482,11 +16630,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="68.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="9" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="69.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="68.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="68.42578125" collapsed="true"/>
+    <col min="4" max="9" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="69.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16604,7 +16752,7 @@
         <v>1431</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -16910,7 +17058,7 @@
         <v>687</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -16928,7 +17076,7 @@
         <v>693</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -16974,8 +17122,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="132" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17072,8 +17220,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17139,8 +17287,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17183,9 +17331,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" style="28" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="28" width="8.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -17242,9 +17390,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -17301,9 +17449,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -17360,7 +17508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -18678,9 +18826,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18737,9 +18885,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18796,9 +18944,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18843,8 +18991,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -18883,8 +19031,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18933,8 +19081,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -18969,8 +19117,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -19026,8 +19174,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -19077,57 +19225,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="72" max="73" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="72" max="73" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.25">
@@ -19423,51 +19571,51 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="41" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="53" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="58" max="59" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="64" max="65" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="22" max="23" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="28" max="29" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="34" max="35" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="40" max="41" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="46" max="47" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="52" max="53" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="58" max="59" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="64" max="65" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
@@ -19710,7 +19858,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -21764,52 +21912,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -22053,52 +22201,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -22342,52 +22490,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -22631,52 +22779,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -22920,52 +23068,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="25" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="55" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="66" max="67" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="28" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="24" max="25" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="36" max="37" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="42" max="43" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="48" max="49" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="54" max="55" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="60" max="61" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="66" max="67" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -23209,8 +23357,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23249,8 +23397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23294,8 +23442,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23339,8 +23487,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23384,8 +23532,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23429,8 +23577,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23507,8 +23655,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23552,8 +23700,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23589,9 +23737,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="24.7109375" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="130" width="12.0" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="130" width="24.7109375" collapsed="true"/>
+    <col min="4" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23657,7 +23805,7 @@
         <v>1431</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -23701,9 +23849,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="20.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="12.0" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23785,9 +23933,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="130" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="130" width="17.5703125" collapsed="true"/>
+    <col min="3" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23870,9 +24018,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="130" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="130" width="12.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23940,8 +24088,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24009,8 +24157,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24080,11 +24228,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -24135,10 +24283,10 @@
         <v>1753</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="E3" s="134" t="s">
         <v>1546</v>
@@ -24169,13 +24317,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -24252,10 +24400,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.85546875" style="28" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="28" width="31.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="45.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24575,13 +24723,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -24658,13 +24806,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -24741,7 +24889,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -24783,7 +24931,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24827,7 +24975,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24863,8 +25011,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -24915,8 +25063,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24966,14 +25114,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="132" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" style="132" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="14.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="132" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="132" width="10.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="132" width="10.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="132" width="11.140625" collapsed="true"/>
+    <col min="8" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -25042,7 +25190,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25132,7 +25280,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25222,9 +25370,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25450,9 +25598,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="28" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="24.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25522,9 +25670,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="28" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="24.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25546,7 +25694,7 @@
         <v>1481</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -25584,7 +25732,7 @@
         <v>1482</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -25611,8 +25759,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25660,9 +25808,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" style="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="28" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="28" width="20.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="28" width="24.42578125" collapsed="true"/>
+    <col min="3" max="16384" style="28" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25684,7 +25832,7 @@
         <v>1489</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -25722,7 +25870,7 @@
         <v>1492</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
   </sheetData>
@@ -25744,17 +25892,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -25893,9 +26041,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="35" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="18.0" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="132" width="35.0" collapsed="true"/>
+    <col min="4" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -26267,9 +26415,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="130" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="130" width="35.0" collapsed="true"/>
+    <col min="3" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -26448,9 +26596,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" style="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="130" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="130" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="130" width="35.0" collapsed="true"/>
+    <col min="3" max="16384" style="130" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -26623,9 +26771,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="30.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -26811,10 +26959,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="132" width="49.42578125" collapsed="true"/>
+    <col min="4" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -27060,9 +27208,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -27288,10 +27436,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.7109375" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.42578125" style="132" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="19.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="30.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="132" width="49.42578125" collapsed="true"/>
+    <col min="4" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -27537,9 +27685,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="28.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27597,9 +27745,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="28.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27668,9 +27816,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="132" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="28.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27739,9 +27887,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.140625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="29.140625" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -27821,9 +27969,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="39.0" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -27910,9 +28058,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="39.0" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -27996,8 +28144,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28041,8 +28189,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28097,8 +28245,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28153,9 +28301,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -28381,8 +28529,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28426,8 +28574,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28482,8 +28630,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -28538,9 +28686,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35" style="132" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="132" width="35.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -28940,9 +29088,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="35" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="18.85546875" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="132" width="35.0" collapsed="true"/>
+    <col min="4" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -29122,9 +29270,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="25.85546875" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -29194,9 +29342,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="25.85546875" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -29258,9 +29406,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" style="132" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="132" width="25.85546875" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -29303,9 +29451,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" style="132" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="132" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="132" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="132" width="18.28515625" collapsed="true"/>
+    <col min="3" max="16384" style="132" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -29348,9 +29496,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="99" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" style="99" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="99" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="99" width="18.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="99" width="35.0" collapsed="true"/>
+    <col min="3" max="16384" style="99" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>